<commit_message>
Dependency Implemented for Edit employee
</commit_message>
<xml_diff>
--- a/Data/ConfigData/EmployeeConfig.xlsx
+++ b/Data/ConfigData/EmployeeConfig.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="39">
   <si>
     <t>TestId</t>
   </si>
@@ -104,7 +104,34 @@
     <t>editemp_001</t>
   </si>
   <si>
+    <t>Permanent Employee Edit</t>
+  </si>
+  <si>
     <t>EditEmp</t>
+  </si>
+  <si>
+    <t>DepEmployee</t>
+  </si>
+  <si>
+    <t>editemp_002</t>
+  </si>
+  <si>
+    <t>editemp_003</t>
+  </si>
+  <si>
+    <t>editemp_004</t>
+  </si>
+  <si>
+    <t>Trainee Employee Edit</t>
+  </si>
+  <si>
+    <t>editemp_005</t>
+  </si>
+  <si>
+    <t>Contractual  Employee Edit</t>
+  </si>
+  <si>
+    <t>editemp_006</t>
   </si>
 </sst>
 </file>
@@ -112,10 +139,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -134,6 +161,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +183,97 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -150,40 +282,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -197,93 +305,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -294,43 +321,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -342,31 +471,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -384,97 +501,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -538,21 +565,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -585,157 +597,173 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1059,7 +1087,7 @@
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4"/>
@@ -1329,19 +1357,19 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6"/>
   <cols>
     <col min="1" max="1" width="13.8571428571429" customWidth="1"/>
     <col min="2" max="2" width="24.5714285714286" customWidth="1"/>
     <col min="3" max="3" width="23.4285714285714" customWidth="1"/>
     <col min="4" max="4" width="10.4285714285714" customWidth="1"/>
-    <col min="5" max="5" width="11.8571428571429" customWidth="1"/>
+    <col min="5" max="5" width="14.4285714285714" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="17.4285714285714" customWidth="1"/>
     <col min="8" max="8" width="15.1428571428571" customWidth="1"/>
@@ -1429,25 +1457,35 @@
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>22</v>
+      <c r="B2" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="2">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
+        <v>3</v>
+      </c>
       <c r="J2" s="2" t="s">
         <v>25</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L2" s="2">
         <v>4</v>
@@ -1462,7 +1500,7 @@
         <v>25</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q2" s="2">
         <v>4</v>
@@ -1481,53 +1519,329 @@
       </c>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="2">
+        <v>6</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>3</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="2">
+        <v>4</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2">
+        <v>3</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>4</v>
+      </c>
+      <c r="R3" s="2">
+        <v>0</v>
+      </c>
+      <c r="S3" s="2">
+        <v>1</v>
+      </c>
+      <c r="T3" s="2">
+        <v>60</v>
+      </c>
+      <c r="U3" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="2">
+        <v>6</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>3</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="2">
+        <v>4</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2">
+        <v>3</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>4</v>
+      </c>
+      <c r="R4" s="2">
+        <v>0</v>
+      </c>
+      <c r="S4" s="2">
+        <v>1</v>
+      </c>
+      <c r="T4" s="2">
+        <v>60</v>
+      </c>
+      <c r="U4" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" customFormat="1" spans="10:10">
-      <c r="J5" s="2"/>
+    <row r="5" customFormat="1" spans="1:21">
+      <c r="A5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="3">
+        <v>6</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>3</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="3">
+        <v>4</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0</v>
+      </c>
+      <c r="N5" s="3">
+        <v>3</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>4</v>
+      </c>
+      <c r="R5" s="3">
+        <v>0</v>
+      </c>
+      <c r="S5" s="3">
+        <v>1</v>
+      </c>
+      <c r="T5" s="3">
+        <v>60</v>
+      </c>
+      <c r="U5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="3">
+        <v>6</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>3</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="3">
+        <v>4</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0</v>
+      </c>
+      <c r="N6" s="3">
+        <v>3</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>4</v>
+      </c>
+      <c r="R6" s="3">
+        <v>0</v>
+      </c>
+      <c r="S6" s="3">
+        <v>1</v>
+      </c>
+      <c r="T6" s="3">
+        <v>60</v>
+      </c>
+      <c r="U6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="3">
+        <v>6</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>3</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="3">
+        <v>4</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0</v>
+      </c>
+      <c r="N7" s="3">
+        <v>3</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>4</v>
+      </c>
+      <c r="R7" s="3">
+        <v>0</v>
+      </c>
+      <c r="S7" s="3">
+        <v>1</v>
+      </c>
+      <c r="T7" s="3">
+        <v>60</v>
+      </c>
+      <c r="U7" s="3">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Edit employee data added
</commit_message>
<xml_diff>
--- a/Data/ConfigData/EmployeeConfig.xlsx
+++ b/Data/ConfigData/EmployeeConfig.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="44">
   <si>
     <t>TestId</t>
   </si>
@@ -104,7 +104,7 @@
     <t>editemp_001</t>
   </si>
   <si>
-    <t>Permanent Employee Edit</t>
+    <t>Edit personal Information of Permanent Employee</t>
   </si>
   <si>
     <t>EditEmp</t>
@@ -116,22 +116,37 @@
     <t>editemp_002</t>
   </si>
   <si>
+    <t>Edit Education Details of Permanent Employee</t>
+  </si>
+  <si>
     <t>editemp_003</t>
   </si>
   <si>
+    <t>Edit Employment Details of Permanent Employee, Probation to Confirm</t>
+  </si>
+  <si>
     <t>editemp_004</t>
   </si>
   <si>
-    <t>Trainee Employee Edit</t>
+    <t>Edit Salary Details of trainee Employee</t>
   </si>
   <si>
     <t>editemp_005</t>
   </si>
   <si>
-    <t>Contractual  Employee Edit</t>
+    <t>Edit Salary Details of Contractual Employee</t>
   </si>
   <si>
     <t>editemp_006</t>
+  </si>
+  <si>
+    <t>Edit Salary Details of Permanent Employee</t>
+  </si>
+  <si>
+    <t>editemp_007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit Employment Details of Permanent Employee, Exit date and employee status change from Active to Resigned </t>
   </si>
 </sst>
 </file>
@@ -140,9 +155,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -169,7 +184,129 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -183,128 +320,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -321,6 +336,78 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -345,6 +432,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -369,7 +468,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -382,126 +517,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -515,13 +530,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -546,6 +565,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -591,31 +619,18 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -633,137 +648,136 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1357,16 +1371,16 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:U7"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="7"/>
   <cols>
     <col min="1" max="1" width="13.8571428571429" customWidth="1"/>
-    <col min="2" max="2" width="24.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="112.857142857143" customWidth="1"/>
     <col min="3" max="3" width="23.4285714285714" customWidth="1"/>
     <col min="4" max="4" width="10.4285714285714" customWidth="1"/>
     <col min="5" max="5" width="14.4285714285714" customWidth="1"/>
@@ -1457,7 +1471,7 @@
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1522,8 +1536,8 @@
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>29</v>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>23</v>
@@ -1585,10 +1599,10 @@
     </row>
     <row r="4" spans="1:21">
       <c r="A4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>23</v>
@@ -1650,196 +1664,261 @@
     </row>
     <row r="5" customFormat="1" spans="1:21">
       <c r="A5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="F5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="2">
         <v>6</v>
       </c>
-      <c r="H5" s="3">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3">
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
         <v>3</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L5" s="3">
-        <v>4</v>
-      </c>
-      <c r="M5" s="3">
-        <v>0</v>
-      </c>
-      <c r="N5" s="3">
+      <c r="K5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="2">
+        <v>4</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
         <v>3</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="O5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="P5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q5" s="3">
-        <v>4</v>
-      </c>
-      <c r="R5" s="3">
-        <v>0</v>
-      </c>
-      <c r="S5" s="3">
-        <v>1</v>
-      </c>
-      <c r="T5" s="3">
+      <c r="P5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>4</v>
+      </c>
+      <c r="R5" s="2">
+        <v>0</v>
+      </c>
+      <c r="S5" s="2">
+        <v>1</v>
+      </c>
+      <c r="T5" s="2">
         <v>60</v>
       </c>
-      <c r="U5" s="3">
+      <c r="U5" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:21">
       <c r="A6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="3">
+      <c r="F6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="2">
         <v>6</v>
       </c>
-      <c r="H6" s="3">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3">
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
         <v>3</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" s="3">
-        <v>4</v>
-      </c>
-      <c r="M6" s="3">
-        <v>0</v>
-      </c>
-      <c r="N6" s="3">
+      <c r="K6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="2">
+        <v>4</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
         <v>3</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="O6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="P6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q6" s="3">
-        <v>4</v>
-      </c>
-      <c r="R6" s="3">
-        <v>0</v>
-      </c>
-      <c r="S6" s="3">
-        <v>1</v>
-      </c>
-      <c r="T6" s="3">
+      <c r="P6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>4</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0</v>
+      </c>
+      <c r="S6" s="2">
+        <v>1</v>
+      </c>
+      <c r="T6" s="2">
         <v>60</v>
       </c>
-      <c r="U6" s="3">
+      <c r="U6" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="3">
+      <c r="F7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="2">
         <v>6</v>
       </c>
-      <c r="H7" s="3">
-        <v>0</v>
-      </c>
-      <c r="I7" s="3">
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
         <v>3</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L7" s="3">
-        <v>4</v>
-      </c>
-      <c r="M7" s="3">
-        <v>0</v>
-      </c>
-      <c r="N7" s="3">
+      <c r="K7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="2">
+        <v>4</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2">
         <v>3</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="O7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="P7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q7" s="3">
-        <v>4</v>
-      </c>
-      <c r="R7" s="3">
-        <v>0</v>
-      </c>
-      <c r="S7" s="3">
-        <v>1</v>
-      </c>
-      <c r="T7" s="3">
+      <c r="P7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>4</v>
+      </c>
+      <c r="R7" s="2">
+        <v>0</v>
+      </c>
+      <c r="S7" s="2">
+        <v>1</v>
+      </c>
+      <c r="T7" s="2">
         <v>60</v>
       </c>
-      <c r="U7" s="3">
+      <c r="U7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="2">
+        <v>6</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>3</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L8" s="2">
+        <v>4</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2">
+        <v>3</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>4</v>
+      </c>
+      <c r="R8" s="2">
+        <v>0</v>
+      </c>
+      <c r="S8" s="2">
+        <v>1</v>
+      </c>
+      <c r="T8" s="2">
+        <v>60</v>
+      </c>
+      <c r="U8" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Json String return Implemented
</commit_message>
<xml_diff>
--- a/Data/ConfigData/EmployeeConfig.xlsx
+++ b/Data/ConfigData/EmployeeConfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="NewEmp" sheetId="1" r:id="rId1"/>
@@ -154,9 +154,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
@@ -191,6 +191,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -206,10 +229,71 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -221,76 +305,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -304,24 +320,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -336,13 +336,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -354,31 +468,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -390,73 +486,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -468,36 +510,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -505,18 +517,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -527,6 +527,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -545,26 +569,28 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -601,32 +627,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -648,130 +648,130 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1100,8 +1100,8 @@
   <sheetPr/>
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4"/>
@@ -1373,8 +1373,8 @@
   <sheetPr/>
   <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="7"/>

</xml_diff>